<commit_message>
Update on Report and Documentation of Deadline1. Items of note: 	-Report needs an image for section 3.0 (verilog module/tb connection) 	-Report needs verilog code added in section 6.0
</commit_message>
<xml_diff>
--- a/Deadline1/Test Bench Documentation.xlsx
+++ b/Deadline1/Test Bench Documentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Bench" sheetId="1" r:id="rId1"/>
-    <sheet name="Alpha Xwalk" sheetId="2" r:id="rId2"/>
+    <sheet name="Behavior" sheetId="2" r:id="rId1"/>
+    <sheet name="Test Bench" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="92">
   <si>
     <t>//Beginning Loop (Assume preselected Test-Logic-Reset)</t>
   </si>
@@ -241,14 +241,73 @@
   </si>
   <si>
     <t>Alpha Assignment</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>clock_ir</t>
+  </si>
+  <si>
+    <t>capture_ir</t>
+  </si>
+  <si>
+    <t>shift_ir</t>
+  </si>
+  <si>
+    <t>update_ir</t>
+  </si>
+  <si>
+    <t>clock_dr</t>
+  </si>
+  <si>
+    <t>capture_dr</t>
+  </si>
+  <si>
+    <t>shift_dr</t>
+  </si>
+  <si>
+    <t>update_dr</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Output Wire Behavior</t>
+  </si>
+  <si>
+    <t>State Details</t>
+  </si>
+  <si>
+    <t>On TMS "0"</t>
+  </si>
+  <si>
+    <t>On TMS "1"</t>
+  </si>
+  <si>
+    <t>Moore State Details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -270,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -287,11 +346,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -306,12 +510,58 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -390,6 +640,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -424,6 +675,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -599,14 +851,566 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="6" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8">
+        <v>1</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8">
+        <v>1</v>
+      </c>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8">
+        <v>1</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8">
+        <v>1</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:O1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" customWidth="1"/>
@@ -614,7 +1418,7 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -629,13 +1433,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -650,7 +1454,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -665,7 +1469,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -680,7 +1484,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -695,7 +1499,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -710,7 +1514,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -725,7 +1529,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -740,7 +1544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -749,13 +1553,13 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -770,7 +1574,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -785,7 +1589,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -800,7 +1604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -815,7 +1619,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -830,7 +1634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -839,13 +1643,13 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -860,7 +1664,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -875,7 +1679,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -890,7 +1694,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -905,7 +1709,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -920,7 +1724,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -935,7 +1739,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -950,7 +1754,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -965,7 +1769,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -980,7 +1784,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -995,7 +1799,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1010,7 +1814,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1025,7 +1829,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1040,7 +1844,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1049,13 +1853,13 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
       <c r="D33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1070,7 +1874,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1085,7 +1889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1100,7 +1904,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1115,7 +1919,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1130,7 +1934,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1145,7 +1949,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1154,13 +1958,13 @@
       </c>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -1175,7 +1979,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1190,7 +1994,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -1205,7 +2009,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1220,7 +2024,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -1235,7 +2039,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1250,7 +2054,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1265,7 +2069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -1280,7 +2084,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -1295,7 +2099,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -1310,7 +2114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -1325,7 +2129,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +2144,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -1355,7 +2159,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -1368,161 +2172,6 @@
       </c>
       <c r="E55" t="s">
         <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1531,12 +2180,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>